<commit_message>
Got Specs and HistogramManager working
generate_stats.py now successfully runs again.

I'm still missing the StatsManager step of actually calculating
statistics on all these histograms, however.  The code has been
translated but it's not yet been tested.
</commit_message>
<xml_diff>
--- a/movement_validation/statistics/better_feature_metadata/features specifications.xlsx
+++ b/movement_validation/statistics/better_feature_metadata/features specifications.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="300">
   <si>
     <t>feature_field</t>
   </si>
@@ -574,114 +574,9 @@
     <t>seconds</t>
   </si>
   <si>
-    <t>posture.coils.event_durations</t>
-  </si>
-  <si>
-    <t>posture.coils.time_between_events</t>
-  </si>
-  <si>
-    <t>posture.coils.distance_between_events</t>
-  </si>
-  <si>
     <t>posture.coils.frequency</t>
   </si>
   <si>
-    <t>posture.coils.time_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.turns.omegas.omegas.event_durations</t>
-  </si>
-  <si>
-    <t>locomotion.turns.omegas.omegas.time_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.turns.omegas.omegas.distance_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.turns.omegas.omegas.frequency</t>
-  </si>
-  <si>
-    <t>locomotion.turns.omegas.omegas.time_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.turns.upsilons.upsilons.event_durations</t>
-  </si>
-  <si>
-    <t>locomotion.turns.upsilons.upsilons.time_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.turns.upsilons.upsilons.distance_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.turns.upsilons.upsilons.frequency</t>
-  </si>
-  <si>
-    <t>locomotion.turns.upsilons.upsilons.time_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.event_durations</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.distance_during_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.time_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.distance_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.frequency</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.time_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.forward.data_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.event_durations</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.distance_during_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.time_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.distance_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.frequency</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.time_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.paused.data_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.event_durations</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.distance_during_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.time_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.distance_between_events</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.frequency</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.time_ratio</t>
-  </si>
-  <si>
-    <t>locomotion.motion_events.backward.data_ratio</t>
-  </si>
-  <si>
     <t>Posture</t>
   </si>
   <si>
@@ -971,6 +866,57 @@
   </si>
   <si>
     <t>InEvent</t>
+  </si>
+  <si>
+    <t>remove_partial_events</t>
+  </si>
+  <si>
+    <t>locomotion.foraging_bends.amplitude</t>
+  </si>
+  <si>
+    <t>locomotion.crawling_bends.head.amplitude</t>
+  </si>
+  <si>
+    <t>locomotion.crawling_bends.midbody.amplitude</t>
+  </si>
+  <si>
+    <t>locomotion.crawling_bends.tail.amplitude</t>
+  </si>
+  <si>
+    <t>locomotion.crawling_bends.head.frequency</t>
+  </si>
+  <si>
+    <t>locomotion.crawling_bends.midbody.frequency</t>
+  </si>
+  <si>
+    <t>locomotion.crawling_bends.tail.frequency</t>
+  </si>
+  <si>
+    <t>locomotion.foraging_bends.angle_speed</t>
+  </si>
+  <si>
+    <t>path.range.value</t>
+  </si>
+  <si>
+    <t>posture.coils</t>
+  </si>
+  <si>
+    <t>locomotion.turns.omegas.omegas</t>
+  </si>
+  <si>
+    <t>locomotion.turns.upsilons.upsilons</t>
+  </si>
+  <si>
+    <t>locomotion.motion_events.forward</t>
+  </si>
+  <si>
+    <t>locomotion.motion_events.paused</t>
+  </si>
+  <si>
+    <t>locomotion.motion_events.backward</t>
+  </si>
+  <si>
+    <t>frequency</t>
   </si>
 </sst>
 </file>
@@ -1338,12 +1284,14 @@
   <dimension ref="A1:Q94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
@@ -1385,7 +1333,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>13</v>
@@ -1394,7 +1342,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>11</v>
+        <v>283</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
@@ -1411,7 +1359,7 @@
         <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>175</v>
@@ -1440,7 +1388,7 @@
         <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
         <v>176</v>
@@ -1469,7 +1417,7 @@
         <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
         <v>177</v>
@@ -1498,7 +1446,7 @@
         <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>178</v>
@@ -1527,7 +1475,7 @@
         <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -1562,7 +1510,7 @@
         <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1597,7 +1545,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
@@ -1632,7 +1580,7 @@
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1667,7 +1615,7 @@
         <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -1702,7 +1650,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1737,7 +1685,7 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -1772,7 +1720,7 @@
         <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -1807,7 +1755,7 @@
         <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1842,7 +1790,7 @@
         <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
@@ -1877,7 +1825,7 @@
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -1912,7 +1860,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -1947,7 +1895,7 @@
         <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C18" t="s">
         <v>36</v>
@@ -1982,7 +1930,7 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C19" t="s">
         <v>37</v>
@@ -2017,7 +1965,7 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -2052,7 +2000,7 @@
         <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -2087,7 +2035,7 @@
         <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C22" t="s">
         <v>40</v>
@@ -2122,7 +2070,7 @@
         <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -2157,7 +2105,7 @@
         <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C24" t="s">
         <v>42</v>
@@ -2192,7 +2140,7 @@
         <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C25" t="s">
         <v>43</v>
@@ -2227,7 +2175,7 @@
         <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C26" t="s">
         <v>44</v>
@@ -2262,7 +2210,7 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -2297,7 +2245,7 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C28" t="s">
         <v>46</v>
@@ -2332,7 +2280,7 @@
         <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C29" t="s">
         <v>47</v>
@@ -2367,7 +2315,7 @@
         <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
@@ -2402,7 +2350,7 @@
         <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C31" t="s">
         <v>49</v>
@@ -2437,7 +2385,7 @@
         <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -2472,7 +2420,7 @@
         <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C33" t="s">
         <v>51</v>
@@ -2499,7 +2447,7 @@
         <v>163</v>
       </c>
       <c r="P33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33">
         <v>1</v>
@@ -2510,7 +2458,7 @@
         <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C34" t="s">
         <v>51</v>
@@ -2537,7 +2485,7 @@
         <v>163</v>
       </c>
       <c r="P34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q34">
         <v>1</v>
@@ -2548,7 +2496,7 @@
         <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C35" t="s">
         <v>51</v>
@@ -2575,7 +2523,7 @@
         <v>163</v>
       </c>
       <c r="P35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q35">
         <v>1</v>
@@ -2586,7 +2534,7 @@
         <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C36" t="s">
         <v>51</v>
@@ -2613,7 +2561,7 @@
         <v>163</v>
       </c>
       <c r="P36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q36">
         <v>1</v>
@@ -2624,7 +2572,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C37" t="s">
         <v>51</v>
@@ -2651,7 +2599,7 @@
         <v>163</v>
       </c>
       <c r="P37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q37">
         <v>1</v>
@@ -2662,7 +2610,7 @@
         <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
         <v>51</v>
@@ -2689,7 +2637,7 @@
         <v>163</v>
       </c>
       <c r="P38">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q38">
         <v>1</v>
@@ -2700,7 +2648,7 @@
         <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C39" t="s">
         <v>52</v>
@@ -2735,7 +2683,7 @@
         <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C40" t="s">
         <v>53</v>
@@ -2770,7 +2718,7 @@
         <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C41" t="s">
         <v>54</v>
@@ -2805,7 +2753,7 @@
         <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
         <v>55</v>
@@ -2840,7 +2788,7 @@
         <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C43" t="s">
         <v>56</v>
@@ -2875,7 +2823,7 @@
         <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C44" t="s">
         <v>57</v>
@@ -2910,7 +2858,7 @@
         <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C45" t="s">
         <v>58</v>
@@ -2945,7 +2893,7 @@
         <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C46" t="s">
         <v>59</v>
@@ -2980,7 +2928,7 @@
         <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C47" t="s">
         <v>60</v>
@@ -3015,7 +2963,7 @@
         <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C48" t="s">
         <v>61</v>
@@ -3050,10 +2998,10 @@
         <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>284</v>
       </c>
       <c r="D49" t="s">
         <v>62</v>
@@ -3085,10 +3033,10 @@
         <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>291</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -3120,10 +3068,10 @@
         <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>285</v>
       </c>
       <c r="D51" t="s">
         <v>64</v>
@@ -3155,10 +3103,10 @@
         <v>72</v>
       </c>
       <c r="B52" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>65</v>
+        <v>286</v>
       </c>
       <c r="D52" t="s">
         <v>65</v>
@@ -3190,10 +3138,10 @@
         <v>72</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>287</v>
       </c>
       <c r="D53" t="s">
         <v>66</v>
@@ -3225,10 +3173,10 @@
         <v>72</v>
       </c>
       <c r="B54" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>288</v>
       </c>
       <c r="D54" t="s">
         <v>67</v>
@@ -3260,10 +3208,10 @@
         <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>289</v>
       </c>
       <c r="D55" t="s">
         <v>68</v>
@@ -3295,10 +3243,10 @@
         <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>290</v>
       </c>
       <c r="D56" t="s">
         <v>69</v>
@@ -3330,10 +3278,10 @@
         <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>292</v>
       </c>
       <c r="D57" t="s">
         <v>70</v>
@@ -3365,7 +3313,7 @@
         <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C58" t="s">
         <v>71</v>
@@ -3400,19 +3348,19 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C59" t="s">
-        <v>185</v>
+        <v>293</v>
       </c>
       <c r="D59" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="E59" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="F59" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="G59">
         <v>0.1</v>
@@ -3427,10 +3375,10 @@
         <v>184</v>
       </c>
       <c r="K59" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="L59" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -3444,19 +3392,19 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>186</v>
+        <v>293</v>
       </c>
       <c r="D60" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="E60" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="F60" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="G60">
         <v>5</v>
@@ -3471,10 +3419,10 @@
         <v>184</v>
       </c>
       <c r="K60" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="L60" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -3488,19 +3436,19 @@
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>293</v>
       </c>
       <c r="D61" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="E61" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="F61" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="G61">
         <v>100</v>
@@ -3512,13 +3460,13 @@
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K61" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="L61" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -3532,19 +3480,19 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>293</v>
       </c>
       <c r="D62" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E62" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="F62" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="G62">
         <v>1E-3</v>
@@ -3557,6 +3505,9 @@
       </c>
       <c r="J62" t="s">
         <v>168</v>
+      </c>
+      <c r="K62" t="s">
+        <v>299</v>
       </c>
       <c r="N62">
         <v>0</v>
@@ -3570,19 +3521,19 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
       <c r="D63" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="E63" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="F63" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G63">
         <v>1E-3</v>
@@ -3594,7 +3545,10 @@
         <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>291</v>
+        <v>256</v>
+      </c>
+      <c r="K63" t="s">
+        <v>274</v>
       </c>
       <c r="N63">
         <v>0</v>
@@ -3608,19 +3562,19 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
+        <v>294</v>
       </c>
       <c r="D64" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="E64" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="F64" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="G64">
         <v>0.1</v>
@@ -3635,13 +3589,13 @@
         <v>184</v>
       </c>
       <c r="K64" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="L64" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="M64" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -3655,19 +3609,19 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>191</v>
+        <v>294</v>
       </c>
       <c r="D65" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="E65" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="F65" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="G65">
         <v>5</v>
@@ -3682,13 +3636,13 @@
         <v>184</v>
       </c>
       <c r="K65" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="L65" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="M65" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -3702,19 +3656,19 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C66" t="s">
+        <v>294</v>
+      </c>
+      <c r="D66" t="s">
         <v>192</v>
       </c>
-      <c r="D66" t="s">
-        <v>227</v>
-      </c>
       <c r="E66" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="F66" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="G66">
         <v>100</v>
@@ -3726,16 +3680,16 @@
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K66" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="L66" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="M66" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -3749,19 +3703,19 @@
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C67" t="s">
+        <v>294</v>
+      </c>
+      <c r="D67" t="s">
         <v>193</v>
       </c>
-      <c r="D67" t="s">
-        <v>228</v>
-      </c>
       <c r="E67" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="F67" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="G67">
         <v>1E-3</v>
@@ -3774,6 +3728,9 @@
       </c>
       <c r="J67" t="s">
         <v>168</v>
+      </c>
+      <c r="K67" t="s">
+        <v>299</v>
       </c>
       <c r="N67">
         <v>0</v>
@@ -3787,19 +3744,19 @@
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C68" t="s">
+        <v>294</v>
+      </c>
+      <c r="D68" t="s">
         <v>194</v>
       </c>
-      <c r="D68" t="s">
-        <v>229</v>
-      </c>
       <c r="E68" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="F68" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G68">
         <v>1E-3</v>
@@ -3811,7 +3768,10 @@
         <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>291</v>
+        <v>256</v>
+      </c>
+      <c r="K68" t="s">
+        <v>274</v>
       </c>
       <c r="N68">
         <v>0</v>
@@ -3825,19 +3785,19 @@
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
+        <v>295</v>
+      </c>
+      <c r="D69" t="s">
         <v>195</v>
       </c>
-      <c r="D69" t="s">
-        <v>230</v>
-      </c>
       <c r="E69" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="F69" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="G69">
         <v>0.1</v>
@@ -3852,13 +3812,13 @@
         <v>184</v>
       </c>
       <c r="K69" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="L69" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="M69" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -3872,19 +3832,19 @@
         <v>16</v>
       </c>
       <c r="B70" t="s">
+        <v>187</v>
+      </c>
+      <c r="C70" t="s">
+        <v>295</v>
+      </c>
+      <c r="D70" t="s">
+        <v>195</v>
+      </c>
+      <c r="E70" t="s">
         <v>222</v>
       </c>
-      <c r="C70" t="s">
-        <v>196</v>
-      </c>
-      <c r="D70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E70" t="s">
-        <v>257</v>
-      </c>
       <c r="F70" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="G70">
         <v>5</v>
@@ -3899,13 +3859,13 @@
         <v>184</v>
       </c>
       <c r="K70" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="L70" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="M70" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -3919,19 +3879,19 @@
         <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C71" t="s">
-        <v>197</v>
+        <v>295</v>
       </c>
       <c r="D71" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="E71" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="F71" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="G71">
         <v>100</v>
@@ -3943,16 +3903,16 @@
         <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K71" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="L71" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="M71" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -3966,19 +3926,19 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C72" t="s">
-        <v>198</v>
+        <v>295</v>
       </c>
       <c r="D72" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="E72" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="F72" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="G72">
         <v>1E-3</v>
@@ -3991,6 +3951,9 @@
       </c>
       <c r="J72" t="s">
         <v>168</v>
+      </c>
+      <c r="K72" t="s">
+        <v>299</v>
       </c>
       <c r="N72">
         <v>0</v>
@@ -4004,19 +3967,19 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C73" t="s">
-        <v>199</v>
+        <v>295</v>
       </c>
       <c r="D73" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="E73" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="F73" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G73">
         <v>1E-3</v>
@@ -4028,7 +3991,10 @@
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>291</v>
+        <v>256</v>
+      </c>
+      <c r="K73" t="s">
+        <v>274</v>
       </c>
       <c r="N73">
         <v>0</v>
@@ -4042,19 +4008,19 @@
         <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C74" t="s">
-        <v>200</v>
+        <v>296</v>
       </c>
       <c r="D74" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="E74" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="F74" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="G74">
         <v>0.5</v>
@@ -4069,10 +4035,10 @@
         <v>184</v>
       </c>
       <c r="K74" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="L74" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -4086,19 +4052,19 @@
         <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C75" t="s">
-        <v>201</v>
+        <v>296</v>
       </c>
       <c r="D75" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="E75" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="F75" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="G75">
         <v>10</v>
@@ -4110,13 +4076,13 @@
         <v>0</v>
       </c>
       <c r="J75" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K75" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="L75" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="N75">
         <v>1</v>
@@ -4130,19 +4096,19 @@
         <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>296</v>
       </c>
       <c r="D76" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="E76" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="F76" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="G76">
         <v>5</v>
@@ -4157,10 +4123,10 @@
         <v>184</v>
       </c>
       <c r="K76" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="L76" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="N76">
         <v>1</v>
@@ -4174,19 +4140,19 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C77" t="s">
-        <v>203</v>
+        <v>296</v>
       </c>
       <c r="D77" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="E77" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="F77" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="G77">
         <v>100</v>
@@ -4198,13 +4164,13 @@
         <v>0</v>
       </c>
       <c r="J77" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K77" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="L77" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="N77">
         <v>1</v>
@@ -4218,19 +4184,19 @@
         <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C78" t="s">
-        <v>204</v>
+        <v>296</v>
       </c>
       <c r="D78" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="E78" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="F78" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="G78">
         <v>1E-3</v>
@@ -4243,6 +4209,9 @@
       </c>
       <c r="J78" t="s">
         <v>168</v>
+      </c>
+      <c r="K78" t="s">
+        <v>299</v>
       </c>
       <c r="N78">
         <v>0</v>
@@ -4256,19 +4225,19 @@
         <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C79" t="s">
-        <v>205</v>
+        <v>296</v>
       </c>
       <c r="D79" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="E79" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="F79" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G79">
         <v>1E-3</v>
@@ -4280,13 +4249,13 @@
         <v>0</v>
       </c>
       <c r="J79" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="K79" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="L79" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N79">
         <v>0</v>
@@ -4300,19 +4269,19 @@
         <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C80" t="s">
-        <v>206</v>
+        <v>296</v>
       </c>
       <c r="D80" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="E80" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="F80" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="G80">
         <v>1E-3</v>
@@ -4324,13 +4293,13 @@
         <v>0</v>
       </c>
       <c r="J80" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="K80" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="L80" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="N80">
         <v>0</v>
@@ -4344,19 +4313,19 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C81" t="s">
-        <v>207</v>
+        <v>297</v>
       </c>
       <c r="D81" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="E81" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="F81" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="G81">
         <v>0.5</v>
@@ -4371,10 +4340,10 @@
         <v>184</v>
       </c>
       <c r="K81" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="L81" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N81">
         <v>1</v>
@@ -4388,19 +4357,19 @@
         <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C82" t="s">
-        <v>208</v>
+        <v>297</v>
       </c>
       <c r="D82" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="E82" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="F82" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="G82">
         <v>10</v>
@@ -4412,13 +4381,13 @@
         <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K82" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="L82" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="N82">
         <v>1</v>
@@ -4432,19 +4401,19 @@
         <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C83" t="s">
-        <v>209</v>
+        <v>297</v>
       </c>
       <c r="D83" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="E83" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="F83" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="G83">
         <v>5</v>
@@ -4459,10 +4428,10 @@
         <v>184</v>
       </c>
       <c r="K83" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="L83" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="N83">
         <v>1</v>
@@ -4476,19 +4445,19 @@
         <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C84" t="s">
-        <v>210</v>
+        <v>297</v>
       </c>
       <c r="D84" t="s">
+        <v>201</v>
+      </c>
+      <c r="E84" t="s">
         <v>236</v>
       </c>
-      <c r="E84" t="s">
-        <v>271</v>
-      </c>
       <c r="F84" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="G84">
         <v>100</v>
@@ -4500,13 +4469,13 @@
         <v>0</v>
       </c>
       <c r="J84" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K84" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="L84" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="N84">
         <v>1</v>
@@ -4520,19 +4489,19 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C85" t="s">
-        <v>211</v>
+        <v>297</v>
       </c>
       <c r="D85" t="s">
+        <v>202</v>
+      </c>
+      <c r="E85" t="s">
         <v>237</v>
       </c>
-      <c r="E85" t="s">
-        <v>272</v>
-      </c>
       <c r="F85" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="G85">
         <v>1E-3</v>
@@ -4545,6 +4514,9 @@
       </c>
       <c r="J85" t="s">
         <v>168</v>
+      </c>
+      <c r="K85" t="s">
+        <v>299</v>
       </c>
       <c r="N85">
         <v>0</v>
@@ -4558,19 +4530,19 @@
         <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C86" t="s">
-        <v>212</v>
+        <v>297</v>
       </c>
       <c r="D86" t="s">
+        <v>203</v>
+      </c>
+      <c r="E86" t="s">
         <v>238</v>
       </c>
-      <c r="E86" t="s">
-        <v>273</v>
-      </c>
       <c r="F86" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G86">
         <v>1E-3</v>
@@ -4582,13 +4554,13 @@
         <v>0</v>
       </c>
       <c r="J86" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="K86" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="L86" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N86">
         <v>0</v>
@@ -4602,19 +4574,19 @@
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C87" t="s">
-        <v>213</v>
+        <v>297</v>
       </c>
       <c r="D87" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="E87" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="F87" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="G87">
         <v>1E-3</v>
@@ -4626,13 +4598,13 @@
         <v>0</v>
       </c>
       <c r="J87" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="K87" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="L87" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="N87">
         <v>0</v>
@@ -4646,19 +4618,19 @@
         <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C88" t="s">
-        <v>214</v>
+        <v>298</v>
       </c>
       <c r="D88" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="E88" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="F88" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="G88">
         <v>0.5</v>
@@ -4673,10 +4645,10 @@
         <v>184</v>
       </c>
       <c r="K88" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="L88" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N88">
         <v>1</v>
@@ -4690,19 +4662,19 @@
         <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C89" t="s">
-        <v>215</v>
+        <v>298</v>
       </c>
       <c r="D89" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="E89" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
       <c r="F89" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="G89">
         <v>10</v>
@@ -4714,13 +4686,13 @@
         <v>0</v>
       </c>
       <c r="J89" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K89" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="L89" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="N89">
         <v>1</v>
@@ -4734,19 +4706,19 @@
         <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="D90" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="E90" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="F90" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="G90">
         <v>5</v>
@@ -4761,10 +4733,10 @@
         <v>184</v>
       </c>
       <c r="K90" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="L90" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="N90">
         <v>1</v>
@@ -4778,19 +4750,19 @@
         <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C91" t="s">
-        <v>217</v>
+        <v>298</v>
       </c>
       <c r="D91" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="E91" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="F91" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="G91">
         <v>100</v>
@@ -4802,13 +4774,13 @@
         <v>0</v>
       </c>
       <c r="J91" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="K91" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="L91" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="N91">
         <v>1</v>
@@ -4822,19 +4794,19 @@
         <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>218</v>
+        <v>298</v>
       </c>
       <c r="D92" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="E92" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="F92" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="G92">
         <v>1E-3</v>
@@ -4847,6 +4819,9 @@
       </c>
       <c r="J92" t="s">
         <v>168</v>
+      </c>
+      <c r="K92" t="s">
+        <v>299</v>
       </c>
       <c r="N92">
         <v>0</v>
@@ -4860,19 +4835,19 @@
         <v>16</v>
       </c>
       <c r="B93" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C93" t="s">
-        <v>219</v>
+        <v>298</v>
       </c>
       <c r="D93" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="E93" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="F93" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G93">
         <v>1E-3</v>
@@ -4884,13 +4859,13 @@
         <v>0</v>
       </c>
       <c r="J93" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="K93" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="L93" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N93">
         <v>0</v>
@@ -4904,19 +4879,19 @@
         <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C94" t="s">
-        <v>220</v>
+        <v>298</v>
       </c>
       <c r="D94" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="E94" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="F94" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="G94">
         <v>1E-3</v>
@@ -4928,13 +4903,13 @@
         <v>0</v>
       </c>
       <c r="J94" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="K94" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="L94" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="N94">
         <v>0</v>
@@ -4952,7 +4927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4965,19 +4942,19 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>316</v>
+        <v>281</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5008,7 +4985,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5028,7 +5005,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -5048,7 +5025,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5068,7 +5045,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -5088,7 +5065,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -5108,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -5128,7 +5105,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -5148,7 +5125,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -5168,7 +5145,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -5182,13 +5159,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -5208,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -5228,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -5242,13 +5219,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>283</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -5268,7 +5245,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -5288,7 +5265,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -5308,7 +5285,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -5345,10 +5322,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>